<commit_message>
Someone updated the master excel file. It wasn't me but going to commit it anyways.
</commit_message>
<xml_diff>
--- a/raw-data/sample_info/Visium_IF_DLPFC_MasterExcel_01262022.xlsx
+++ b/raw-data/sample_info/Visium_IF_DLPFC_MasterExcel_01262022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Neural_Plasticity/TeamIMG/VisiumIF_DLPFC/20220126_VIF_DLPFC_Real/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/h7/32q988ts46nf0kdx_s4kpmx80000gn/T/ch.sudo.cyberduck/23398a3b-e999-488c-ac41-0fd1ea9c81ff/dcs04/lieber/lcolladotor/spatialDLPFC_LIBD4035/spatialDLPFC/raw-data/sample_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C65245-EF49-DC49-A52E-4F706210D573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA49B955-212B-2547-AE5F-C3B879C62B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="2820" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{F167968C-0496-B948-8B0F-AD6F54102453}"/>
+    <workbookView xWindow="31660" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{F167968C-0496-B948-8B0F-AD6F54102453}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>Sample #</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>DLPFC_Post</t>
-  </si>
-  <si>
-    <t>V10B01-107</t>
   </si>
   <si>
     <t xml:space="preserve">Will be Sequenced? </t>
@@ -222,6 +219,12 @@
   </si>
   <si>
     <t>BrNum</t>
+  </si>
+  <si>
+    <t>V10B01-087</t>
+  </si>
+  <si>
+    <t>Note: Previously written V01B01-107 and was corrected on 03/10/2022 to V01B01-087</t>
   </si>
 </sst>
 </file>
@@ -550,17 +553,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,9 +572,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,9 +637,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,12 +648,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -671,11 +656,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1469,10 +1475,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1502,410 +1508,415 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="V2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="W2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="X2" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="20">
+      <c r="A3" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="17">
         <v>1</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="17">
         <v>2720</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="21" t="s">
+      <c r="E3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="19">
         <v>15.69</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="19">
         <v>16</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="19">
         <v>11977.7</v>
       </c>
-      <c r="K3" s="22">
+      <c r="K3" s="19">
         <f>J3*40/1000</f>
         <v>479.108</v>
       </c>
-      <c r="L3" s="22">
+      <c r="L3" s="19">
         <f>K3*0.25</f>
         <v>119.777</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="18">
         <v>16</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="20">
         <v>445</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="21">
         <v>3531.46</v>
       </c>
-      <c r="P3" s="24">
+      <c r="P3" s="21">
         <v>10</v>
       </c>
-      <c r="Q3" s="24">
+      <c r="Q3" s="21">
         <f>O3*P3</f>
         <v>35314.6</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="26" t="s">
+      <c r="S3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="26" t="s">
+      <c r="T3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="26" t="s">
+      <c r="U3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="21">
+      <c r="V3" s="18">
         <v>65</v>
       </c>
-      <c r="W3" s="21">
+      <c r="W3" s="18">
         <f>((V3/100)*5000*50000)</f>
         <v>162500000</v>
       </c>
-      <c r="X3" s="25">
+      <c r="X3" s="22">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4">
+      <c r="A4" s="38"/>
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>6432</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>15.06</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>15</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="4">
         <v>7228.0999999999995</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="4">
         <f t="shared" ref="K4:K6" si="0">J4*40/1000</f>
         <v>289.12400000000002</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="4">
         <f t="shared" ref="L4:L6" si="1">K4*0.25</f>
         <v>72.281000000000006</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="3">
         <v>16</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="3">
         <v>436</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="5">
         <v>2126.04</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="5">
         <v>10</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="5">
         <f t="shared" ref="Q4:Q6" si="2">O4*P4</f>
         <v>21260.400000000001</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="27" t="s">
+      <c r="S4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="27" t="s">
+      <c r="T4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="27" t="s">
+      <c r="U4" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="5">
+      <c r="V4" s="3">
         <v>80</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W4" s="3">
         <f>(V4/100)*5000*50000</f>
         <v>200000000</v>
       </c>
-      <c r="X4" s="8">
+      <c r="X4" s="6">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4">
+      <c r="A5" s="38"/>
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>6522</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="E5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>15.04</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="4">
         <v>15</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="4">
         <v>6083.7</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="4">
         <f t="shared" si="0"/>
         <v>243.34800000000001</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="4">
         <f t="shared" si="1"/>
         <v>60.837000000000003</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="3">
         <v>16</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="3">
         <v>450</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="5">
         <v>2900.14</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="5">
         <v>10</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="5">
         <f t="shared" si="2"/>
         <v>29001.399999999998</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S5" s="27" t="s">
+      <c r="S5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="27" t="s">
+      <c r="T5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="U5" s="27" t="s">
+      <c r="U5" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5" s="3">
         <v>90</v>
       </c>
-      <c r="W5" s="5">
+      <c r="W5" s="3">
         <f t="shared" ref="W5:W6" si="3">(V5/100)*5000*50000</f>
         <v>225000000</v>
       </c>
-      <c r="X5" s="8">
+      <c r="X5" s="6">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10">
+      <c r="A6" s="39"/>
+      <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>8667</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>14.51</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="9">
         <v>15</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="9">
         <v>11729.6</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="9">
         <f t="shared" si="0"/>
         <v>469.18400000000003</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="9">
         <f t="shared" si="1"/>
         <v>117.29600000000001</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="8">
         <v>16</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="8">
         <v>439</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="10">
         <v>3325.52</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="10">
         <v>10</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="10">
         <f t="shared" si="2"/>
         <v>33255.199999999997</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="T6" s="28" t="s">
+      <c r="T6" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="U6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="V6" s="11">
+      <c r="V6" s="8">
         <v>90</v>
       </c>
-      <c r="W6" s="11">
+      <c r="W6" s="8">
         <f t="shared" si="3"/>
         <v>225000000</v>
       </c>
-      <c r="X6" s="15">
+      <c r="X6" s="12">
         <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="E8" s="44" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1923,7 +1934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9970DA7-DA1C-C647-90D7-73EA9589ADBE}">
   <dimension ref="M2:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
@@ -1931,273 +1942,273 @@
   <sheetData>
     <row r="2" spans="13:20" x14ac:dyDescent="0.2">
       <c r="P2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q2" s="36" t="s">
         <v>58</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M3" s="38" t="s">
-        <v>50</v>
+      <c r="M3" s="40" t="s">
+        <v>49</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="O3" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="37" t="s">
+      <c r="P3" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="S3" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="T3" s="38" t="s">
+      <c r="T3" s="40" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="13:20" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M4" s="38"/>
+      <c r="M4" s="40"/>
       <c r="N4" s="43"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="38"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="40"/>
     </row>
     <row r="5" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M5" s="35">
+      <c r="M5" s="31">
         <v>1</v>
       </c>
-      <c r="N5" s="35">
+      <c r="N5" s="31">
         <v>2720</v>
       </c>
-      <c r="O5" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="33">
+      <c r="O5" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="29">
         <v>9868.51</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q5" s="31">
         <f>P5*1</f>
         <v>9868.51</v>
       </c>
-      <c r="R5" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="S5" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="T5" s="41" t="s">
-        <v>55</v>
+      <c r="R5" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="S5" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M6" s="35">
+      <c r="M6" s="31">
         <v>2</v>
       </c>
-      <c r="N6" s="35">
+      <c r="N6" s="31">
         <v>6432</v>
       </c>
-      <c r="O6" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="33">
+      <c r="O6" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="29">
         <v>4767.17</v>
       </c>
-      <c r="Q6" s="35">
+      <c r="Q6" s="31">
         <f t="shared" ref="Q6:Q8" si="0">P6*1</f>
         <v>4767.17</v>
       </c>
-      <c r="R6" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="S6" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="T6" s="41" t="s">
-        <v>55</v>
+      <c r="R6" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="S6" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="T6" s="35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M7" s="35">
+      <c r="M7" s="31">
         <v>3</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="31">
         <v>6522</v>
       </c>
-      <c r="O7" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="P7" s="33">
+      <c r="O7" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7" s="29">
         <v>5108.5</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="Q7" s="31">
         <f t="shared" si="0"/>
         <v>5108.5</v>
       </c>
-      <c r="R7" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="S7" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" s="41" t="s">
-        <v>55</v>
+      <c r="R7" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="S7" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="T7" s="35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M8" s="35">
+      <c r="M8" s="31">
         <v>4</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="31">
         <v>8667</v>
       </c>
-      <c r="O8" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="P8" s="33">
+      <c r="O8" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="P8" s="29">
         <v>8892.94</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="31">
         <f t="shared" si="0"/>
         <v>8892.94</v>
       </c>
-      <c r="R8" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="S8" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="T8" s="41" t="s">
-        <v>55</v>
+      <c r="R8" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="S8" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" s="35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M9" s="35">
+      <c r="M9" s="31">
         <v>5</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="31">
         <v>2720</v>
       </c>
-      <c r="O9" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="P9" s="33">
+      <c r="O9" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" s="29">
         <v>2395.54</v>
       </c>
-      <c r="Q9" s="35">
+      <c r="Q9" s="31">
         <f>P9*5</f>
         <v>11977.7</v>
       </c>
-      <c r="R9" s="33">
+      <c r="R9" s="29">
         <f>Q9*40/1000</f>
         <v>479.108</v>
       </c>
-      <c r="S9" s="33">
+      <c r="S9" s="29">
         <f>R9*0.25</f>
         <v>119.777</v>
       </c>
-      <c r="T9" s="34">
+      <c r="T9" s="30">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M10" s="35">
+      <c r="M10" s="31">
         <v>6</v>
       </c>
-      <c r="N10" s="35">
+      <c r="N10" s="31">
         <v>6432</v>
       </c>
-      <c r="O10" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="P10" s="33">
+      <c r="O10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" s="29">
         <v>1445.62</v>
       </c>
-      <c r="Q10" s="35">
+      <c r="Q10" s="31">
         <f t="shared" ref="Q10:Q12" si="1">P10*5</f>
         <v>7228.0999999999995</v>
       </c>
-      <c r="R10" s="33">
+      <c r="R10" s="29">
         <f t="shared" ref="R10:R12" si="2">Q10*40/1000</f>
         <v>289.12400000000002</v>
       </c>
-      <c r="S10" s="33">
+      <c r="S10" s="29">
         <f t="shared" ref="S10:S12" si="3">R10*0.25</f>
         <v>72.281000000000006</v>
       </c>
-      <c r="T10" s="34">
+      <c r="T10" s="30">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M11" s="35">
+      <c r="M11" s="31">
         <v>7</v>
       </c>
-      <c r="N11" s="35">
+      <c r="N11" s="31">
         <v>6522</v>
       </c>
-      <c r="O11" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="P11" s="33">
+      <c r="O11" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="P11" s="29">
         <v>1216.74</v>
       </c>
-      <c r="Q11" s="35">
+      <c r="Q11" s="31">
         <f t="shared" si="1"/>
         <v>6083.7</v>
       </c>
-      <c r="R11" s="33">
+      <c r="R11" s="29">
         <f t="shared" si="2"/>
         <v>243.34800000000001</v>
       </c>
-      <c r="S11" s="33">
+      <c r="S11" s="29">
         <f t="shared" si="3"/>
         <v>60.837000000000003</v>
       </c>
-      <c r="T11" s="34">
+      <c r="T11" s="30">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="13:20" x14ac:dyDescent="0.2">
-      <c r="M12" s="35">
+      <c r="M12" s="31">
         <v>8</v>
       </c>
-      <c r="N12" s="35">
+      <c r="N12" s="31">
         <v>8667</v>
       </c>
-      <c r="O12" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="P12" s="33">
+      <c r="O12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12" s="29">
         <v>2345.92</v>
       </c>
-      <c r="Q12" s="35">
+      <c r="Q12" s="31">
         <f t="shared" si="1"/>
         <v>11729.6</v>
       </c>
-      <c r="R12" s="33">
+      <c r="R12" s="29">
         <f t="shared" si="2"/>
         <v>469.18400000000003</v>
       </c>
-      <c r="S12" s="33">
+      <c r="S12" s="29">
         <f t="shared" si="3"/>
         <v>117.29600000000001</v>
       </c>
-      <c r="T12" s="34">
+      <c r="T12" s="30">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Drop extra heading that otherwise messes up reading the column names
</commit_message>
<xml_diff>
--- a/raw-data/sample_info/Visium_IF_DLPFC_MasterExcel_01262022.xlsx
+++ b/raw-data/sample_info/Visium_IF_DLPFC_MasterExcel_01262022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/h7/32q988ts46nf0kdx_s4kpmx80000gn/T/ch.sudo.cyberduck/23398a3b-e999-488c-ac41-0fd1ea9c81ff/dcs04/lieber/lcolladotor/spatialDLPFC_LIBD4035/spatialDLPFC/raw-data/sample_info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leocollado/Dropbox/Code/spatialDLPFC/raw-data/sample_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA49B955-212B-2547-AE5F-C3B879C62B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE7E1EC-B6B7-554A-A105-6FED09C36188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31660" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{F167968C-0496-B948-8B0F-AD6F54102453}"/>
+    <workbookView xWindow="23560" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{F167968C-0496-B948-8B0F-AD6F54102453}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>Sample #</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t xml:space="preserve">Est. Read Pairs </t>
-  </si>
-  <si>
-    <t>Sample Sheet</t>
   </si>
   <si>
     <t>Experiment #</t>
@@ -231,7 +228,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -253,15 +250,6 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +259,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -435,15 +423,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -553,88 +532,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -656,8 +635,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -679,9 +658,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,13 +682,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>25496</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>22184</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -750,13 +726,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -821,13 +797,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -892,13 +868,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -963,13 +939,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1034,13 +1010,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>28917</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1475,10 +1451,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1507,422 +1483,394 @@
     <col min="24" max="24" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="17">
+        <v>1</v>
+      </c>
+      <c r="C2" s="17">
+        <v>2720</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="13" t="s">
+      <c r="H2" s="19">
+        <v>15.69</v>
+      </c>
+      <c r="I2" s="19">
+        <v>16</v>
+      </c>
+      <c r="J2" s="19">
+        <v>11977.7</v>
+      </c>
+      <c r="K2" s="19">
+        <f>J2*40/1000</f>
+        <v>479.108</v>
+      </c>
+      <c r="L2" s="19">
+        <f>K2*0.25</f>
+        <v>119.777</v>
+      </c>
+      <c r="M2" s="18">
+        <v>16</v>
+      </c>
+      <c r="N2" s="20">
+        <v>445</v>
+      </c>
+      <c r="O2" s="21">
+        <v>3531.46</v>
+      </c>
+      <c r="P2" s="21">
         <v>10</v>
       </c>
-      <c r="Q2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="W2" s="13" t="s">
+      <c r="Q2" s="21">
+        <f>O2*P2</f>
+        <v>35314.6</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="18">
+        <v>65</v>
+      </c>
+      <c r="W2" s="18">
+        <f>((V2/100)*5000*50000)</f>
+        <v>162500000</v>
+      </c>
+      <c r="X2" s="22">
         <v>39</v>
-      </c>
-      <c r="X2" s="16" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="17">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17">
-        <v>2720</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="19">
-        <v>15.69</v>
-      </c>
-      <c r="I3" s="19">
+      <c r="A3" s="38"/>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6432</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="4">
+        <v>15.06</v>
+      </c>
+      <c r="I3" s="4">
+        <v>15</v>
+      </c>
+      <c r="J3" s="4">
+        <v>7228.0999999999995</v>
+      </c>
+      <c r="K3" s="4">
+        <f t="shared" ref="K3:K5" si="0">J3*40/1000</f>
+        <v>289.12400000000002</v>
+      </c>
+      <c r="L3" s="4">
+        <f t="shared" ref="L3:L5" si="1">K3*0.25</f>
+        <v>72.281000000000006</v>
+      </c>
+      <c r="M3" s="3">
         <v>16</v>
       </c>
-      <c r="J3" s="19">
-        <v>11977.7</v>
-      </c>
-      <c r="K3" s="19">
-        <f>J3*40/1000</f>
-        <v>479.108</v>
-      </c>
-      <c r="L3" s="19">
-        <f>K3*0.25</f>
-        <v>119.777</v>
-      </c>
-      <c r="M3" s="18">
-        <v>16</v>
-      </c>
-      <c r="N3" s="20">
-        <v>445</v>
-      </c>
-      <c r="O3" s="21">
-        <v>3531.46</v>
-      </c>
-      <c r="P3" s="21">
+      <c r="N3" s="3">
+        <v>436</v>
+      </c>
+      <c r="O3" s="5">
+        <v>2126.04</v>
+      </c>
+      <c r="P3" s="5">
         <v>10</v>
       </c>
-      <c r="Q3" s="21">
-        <f>O3*P3</f>
-        <v>35314.6</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="V3" s="18">
-        <v>65</v>
-      </c>
-      <c r="W3" s="18">
-        <f>((V3/100)*5000*50000)</f>
-        <v>162500000</v>
-      </c>
-      <c r="X3" s="22">
+      <c r="Q3" s="5">
+        <f t="shared" ref="Q3:Q5" si="2">O3*P3</f>
+        <v>21260.400000000001</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="V3" s="3">
+        <v>80</v>
+      </c>
+      <c r="W3" s="3">
+        <f>(V3/100)*5000*50000</f>
+        <v>200000000</v>
+      </c>
+      <c r="X3" s="6">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="38"/>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>6432</v>
+        <v>6522</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="4">
-        <v>15.06</v>
+        <v>15.04</v>
       </c>
       <c r="I4" s="4">
         <v>15</v>
       </c>
       <c r="J4" s="4">
-        <v>7228.0999999999995</v>
+        <v>6083.7</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" ref="K4:K6" si="0">J4*40/1000</f>
-        <v>289.12400000000002</v>
+        <f t="shared" si="0"/>
+        <v>243.34800000000001</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L6" si="1">K4*0.25</f>
-        <v>72.281000000000006</v>
+        <f t="shared" si="1"/>
+        <v>60.837000000000003</v>
       </c>
       <c r="M4" s="3">
         <v>16</v>
       </c>
       <c r="N4" s="3">
-        <v>436</v>
+        <v>450</v>
       </c>
       <c r="O4" s="5">
-        <v>2126.04</v>
+        <v>2900.14</v>
       </c>
       <c r="P4" s="5">
         <v>10</v>
       </c>
       <c r="Q4" s="5">
-        <f t="shared" ref="Q4:Q6" si="2">O4*P4</f>
-        <v>21260.400000000001</v>
+        <f t="shared" si="2"/>
+        <v>29001.399999999998</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="S4" s="24" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="T4" s="24" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="U4" s="24" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="V4" s="3">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="W4" s="3">
-        <f>(V4/100)*5000*50000</f>
-        <v>200000000</v>
+        <f t="shared" ref="W4:W5" si="3">(V4/100)*5000*50000</f>
+        <v>225000000</v>
       </c>
       <c r="X4" s="6">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="38"/>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>6522</v>
-      </c>
-      <c r="D5" s="27" t="s">
+    <row r="5" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="7">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7">
+        <v>8667</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="4">
-        <v>15.04</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="E5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="9">
+        <v>14.51</v>
+      </c>
+      <c r="I5" s="9">
         <v>15</v>
       </c>
-      <c r="J5" s="4">
-        <v>6083.7</v>
-      </c>
-      <c r="K5" s="4">
-        <f t="shared" si="0"/>
-        <v>243.34800000000001</v>
-      </c>
-      <c r="L5" s="4">
-        <f t="shared" si="1"/>
-        <v>60.837000000000003</v>
-      </c>
-      <c r="M5" s="3">
-        <v>16</v>
-      </c>
-      <c r="N5" s="3">
-        <v>450</v>
-      </c>
-      <c r="O5" s="5">
-        <v>2900.14</v>
-      </c>
-      <c r="P5" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q5" s="5">
-        <f t="shared" si="2"/>
-        <v>29001.399999999998</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S5" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="U5" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="V5" s="3">
-        <v>90</v>
-      </c>
-      <c r="W5" s="3">
-        <f t="shared" ref="W5:W6" si="3">(V5/100)*5000*50000</f>
-        <v>225000000</v>
-      </c>
-      <c r="X5" s="6">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="7">
-        <v>4</v>
-      </c>
-      <c r="C6" s="7">
-        <v>8667</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="9">
-        <v>14.51</v>
-      </c>
-      <c r="I6" s="9">
-        <v>15</v>
-      </c>
-      <c r="J6" s="9">
+      <c r="J5" s="9">
         <v>11729.6</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K5" s="9">
         <f t="shared" si="0"/>
         <v>469.18400000000003</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L5" s="9">
         <f t="shared" si="1"/>
         <v>117.29600000000001</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M5" s="8">
         <v>16</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N5" s="8">
         <v>439</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O5" s="10">
         <v>3325.52</v>
       </c>
-      <c r="P6" s="10">
+      <c r="P5" s="10">
         <v>10</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="Q5" s="10">
         <f t="shared" si="2"/>
         <v>33255.199999999997</v>
       </c>
-      <c r="R6" s="8" t="s">
+      <c r="R5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="S5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="T6" s="25" t="s">
+      <c r="T5" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="U5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="V6" s="8">
+      <c r="V5" s="8">
         <v>90</v>
       </c>
-      <c r="W6" s="8">
+      <c r="W5" s="8">
         <f t="shared" si="3"/>
         <v>225000000</v>
       </c>
-      <c r="X6" s="12">
+      <c r="X5" s="12">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="E8" s="44" t="s">
-        <v>61</v>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="E7" s="36" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:X1"/>
-    <mergeCell ref="A3:A6"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1942,33 +1890,33 @@
   <sheetData>
     <row r="2" spans="13:20" x14ac:dyDescent="0.2">
       <c r="P2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="13:20" x14ac:dyDescent="0.2">
       <c r="M3" s="40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O3" s="40" t="s">
         <v>10</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R3" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="41" t="s">
         <v>55</v>
-      </c>
-      <c r="S3" s="41" t="s">
-        <v>56</v>
       </c>
       <c r="T3" s="40" t="s">
         <v>7</v>
@@ -1979,10 +1927,10 @@
       <c r="N4" s="43"/>
       <c r="O4" s="40"/>
       <c r="P4" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R4" s="41"/>
       <c r="S4" s="41"/>
@@ -1996,7 +1944,7 @@
         <v>2720</v>
       </c>
       <c r="O5" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P5" s="29">
         <v>9868.51</v>
@@ -2006,13 +1954,13 @@
         <v>9868.51</v>
       </c>
       <c r="R5" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S5" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T5" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="13:20" x14ac:dyDescent="0.2">
@@ -2023,7 +1971,7 @@
         <v>6432</v>
       </c>
       <c r="O6" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P6" s="29">
         <v>4767.17</v>
@@ -2033,13 +1981,13 @@
         <v>4767.17</v>
       </c>
       <c r="R6" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S6" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T6" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="13:20" x14ac:dyDescent="0.2">
@@ -2050,7 +1998,7 @@
         <v>6522</v>
       </c>
       <c r="O7" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P7" s="29">
         <v>5108.5</v>
@@ -2060,13 +2008,13 @@
         <v>5108.5</v>
       </c>
       <c r="R7" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S7" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T7" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="13:20" x14ac:dyDescent="0.2">
@@ -2077,7 +2025,7 @@
         <v>8667</v>
       </c>
       <c r="O8" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P8" s="29">
         <v>8892.94</v>
@@ -2087,13 +2035,13 @@
         <v>8892.94</v>
       </c>
       <c r="R8" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S8" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T8" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="13:20" x14ac:dyDescent="0.2">
@@ -2104,7 +2052,7 @@
         <v>2720</v>
       </c>
       <c r="O9" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P9" s="29">
         <v>2395.54</v>
@@ -2133,7 +2081,7 @@
         <v>6432</v>
       </c>
       <c r="O10" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P10" s="29">
         <v>1445.62</v>
@@ -2162,7 +2110,7 @@
         <v>6522</v>
       </c>
       <c r="O11" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P11" s="29">
         <v>1216.74</v>
@@ -2191,7 +2139,7 @@
         <v>8667</v>
       </c>
       <c r="O12" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P12" s="29">
         <v>2345.92</v>

</xml_diff>